<commit_message>
change column names and year
</commit_message>
<xml_diff>
--- a/data/2011-2012/chart1_2011.xlsx
+++ b/data/2011-2012/chart1_2011.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazeldespain/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hazeldespain/Desktop/TouristData/data/2011-2012/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{574034E5-3444-DF4E-AE21-FC8501E1B7A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20878BD-D6FB-EB4C-82B0-AE30C03DBE9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7440" yWindow="460" windowWidth="14800" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>London</t>
   </si>
@@ -77,15 +77,6 @@
     <t>Tokyo</t>
   </si>
   <si>
-    <t>rank</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>number_visitors</t>
-  </si>
-  <si>
     <t>Vienna</t>
   </si>
   <si>
@@ -96,6 +87,18 @@
   </si>
   <si>
     <t>Kuala Lumpur</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>City Name</t>
+  </si>
+  <si>
+    <t>Overnight International Visitors (Millions)</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -139,7 +142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,30 +457,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F81863-1FD9-8642-9AD5-E8497AB14F82}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -487,8 +493,11 @@
       <c r="C2" s="1">
         <v>20.100000000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -498,8 +507,11 @@
       <c r="C3">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -509,8 +521,11 @@
       <c r="C4">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -520,8 +535,11 @@
       <c r="C5">
         <v>11.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -531,8 +549,11 @@
       <c r="C6">
         <v>10.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -542,8 +563,11 @@
       <c r="C7">
         <v>10.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -553,8 +577,11 @@
       <c r="C8" s="2">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -564,8 +591,11 @@
       <c r="C9">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -575,8 +605,11 @@
       <c r="C10">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -586,8 +619,11 @@
       <c r="C11">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -597,8 +633,11 @@
       <c r="C12">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -608,41 +647,53 @@
       <c r="C13">
         <v>7.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C14">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -652,19 +703,25 @@
       <c r="C17">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C18">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -674,8 +731,11 @@
       <c r="C19">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>9</v>
       </c>
@@ -685,8 +745,11 @@
       <c r="C20">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -695,6 +758,9 @@
       </c>
       <c r="C21" s="3">
         <v>5</v>
+      </c>
+      <c r="D21">
+        <v>2010</v>
       </c>
     </row>
   </sheetData>

</xml_diff>